<commit_message>
added k=10 comment, updated excel file
</commit_message>
<xml_diff>
--- a/packages/src/assign10/klargestplots.xlsx
+++ b/packages/src/assign10/klargestplots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viviv\Documents\GitHub\cs2420-assignments\packages\src\assign10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E20BC73D-4BCA-4E03-B3A3-DF1E7B8239FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA814216-378A-4640-BD5B-80B59F93499A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A197148-E2D3-4F29-9AD2-A9E2594D99F6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>k=1</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>k=N/2</t>
+  </si>
+  <si>
+    <t>k=10</t>
   </si>
 </sst>
 </file>
@@ -202,138 +205,143 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>60000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>70000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>80000</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>90000</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>110000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>120000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>130000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>140000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>150000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>160000</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>170000</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>180000</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>190000</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>200000</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$21</c:f>
+              <c:f>Sheet1!$B$1:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1843130</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1699930</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>2043010</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>971930</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2814570</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1773170</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1880920</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2920750</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>2839610</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>4086380</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>4869290</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>5032120</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>5913980</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>8518640</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>6982800</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>6263810</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="0.00E+00">
+                <c:pt idx="17" formatCode="0.00E+00">
                   <c:v>11720280</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>8323540</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>8969620</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="0.00E+00">
+                <c:pt idx="20" formatCode="0.00E+00">
                   <c:v>12740360</c:v>
                 </c:pt>
               </c:numCache>
@@ -372,138 +380,143 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>60000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>70000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>80000</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>90000</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>110000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>120000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>130000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>140000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>150000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>160000</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>170000</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>180000</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>190000</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>200000</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$21</c:f>
+              <c:f>Sheet1!$C$1:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3471420</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>6966620</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3361440</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1818060</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2097980</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>2072530</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2840700</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3994200</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>4521150</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>5639000</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
+                <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>15089810</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>8018970</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="0.00E+00">
+                <c:pt idx="13" formatCode="0.00E+00">
                   <c:v>29609090</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>9703870</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.00E+00">
+                <c:pt idx="15" formatCode="0.00E+00">
                   <c:v>10746250</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="0.00E+00">
+                <c:pt idx="16" formatCode="0.00E+00">
                   <c:v>10183510</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="0.00E+00">
+                <c:pt idx="17" formatCode="0.00E+00">
                   <c:v>13754410</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="0.00E+00">
+                <c:pt idx="18" formatCode="0.00E+00">
                   <c:v>12723970</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="0.00E+00">
+                <c:pt idx="19" formatCode="0.00E+00">
                   <c:v>15094580</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="0.00E+00">
+                <c:pt idx="20" formatCode="0.00E+00">
                   <c:v>18263380</c:v>
                 </c:pt>
               </c:numCache>
@@ -542,138 +555,143 @@
             </c:spPr>
           </c:marker>
           <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$A$2:$A$21</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>20000</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>30000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>40000</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>50000</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>60000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>70000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>80000</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>90000</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>100000</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>110000</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>120000</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>130000</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>140000</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="15">
                   <c:v>150000</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
                   <c:v>160000</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="17">
                   <c:v>170000</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="18">
                   <c:v>180000</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="19">
                   <c:v>190000</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="20">
                   <c:v>200000</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$21</c:f>
+              <c:f>Sheet1!$D$1:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2951410</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>3785830</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>3090490</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>2530690</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2695580</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3460310</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3672300</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>4668330</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>7091910</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>6365950</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="0.00E+00">
+                <c:pt idx="11" formatCode="0.00E+00">
                   <c:v>10200350</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>8711210</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="0.00E+00">
+                <c:pt idx="13" formatCode="0.00E+00">
                   <c:v>10598160</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>9733400</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="0.00E+00">
+                <c:pt idx="15" formatCode="0.00E+00">
                   <c:v>12286210</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="0.00E+00">
+                <c:pt idx="16" formatCode="0.00E+00">
                   <c:v>17591560</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="0.00E+00">
+                <c:pt idx="17" formatCode="0.00E+00">
                   <c:v>16782940</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="0.00E+00">
+                <c:pt idx="18" formatCode="0.00E+00">
                   <c:v>22357220</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="0.00E+00">
+                <c:pt idx="19" formatCode="0.00E+00">
                   <c:v>29298090</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="0.00E+00">
+                <c:pt idx="20" formatCode="0.00E+00">
                   <c:v>29363270</c:v>
                 </c:pt>
               </c:numCache>
@@ -683,6 +701,181 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-FA59-41E3-9FE3-F3EBCE39B009}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$A$1:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>Sort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$1:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2518580</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1267030</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1938220</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>875880</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1416290</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1477660</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1823040</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2197880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2303450</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2539160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3487350</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3960920</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5314110</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4837220</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4866130</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5441180</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6135550</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7186640</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6822590</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7430620</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1C95-4598-9523-0533EE088A1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1522,6 +1715,187 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>k=10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>150000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>190000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>2662090</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1368520</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>804000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1076130</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3365950</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2465300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3141570</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2240380</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2467080</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2847210</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7391610</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4860750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4207670</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6618730</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6678270</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7236720</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="0.00E+00">
+                  <c:v>13946480</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7553610</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9107510</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="0.00E+00">
+                  <c:v>10107810</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-743F-4E62-AC7B-64EB0CB27605}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2856,16 +3230,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>393699</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>58736</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>450849</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>112711</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>384174</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>146049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2892,16 +3266,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>87312</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>134937</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>125412</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>173037</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3228,13 +3602,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AD796C5-737F-4414-9B50-934D43E8244E}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26:M27"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3247,6 +3621,9 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
@@ -3259,8 +3636,11 @@
       <c r="I1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10000</v>
       </c>
@@ -3273,6 +3653,9 @@
       <c r="D2">
         <v>2951410</v>
       </c>
+      <c r="E2">
+        <v>2518580</v>
+      </c>
       <c r="F2">
         <v>10000</v>
       </c>
@@ -3285,8 +3668,11 @@
       <c r="I2" s="1">
         <v>11609900</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2">
+        <v>2662090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>20000</v>
       </c>
@@ -3299,6 +3685,9 @@
       <c r="D3">
         <v>3785830</v>
       </c>
+      <c r="E3">
+        <v>1267030</v>
+      </c>
       <c r="F3">
         <v>20000</v>
       </c>
@@ -3311,8 +3700,11 @@
       <c r="I3">
         <v>7683850</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3">
+        <v>1368520</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>30000</v>
       </c>
@@ -3325,6 +3717,9 @@
       <c r="D4">
         <v>3090490</v>
       </c>
+      <c r="E4">
+        <v>1938220</v>
+      </c>
       <c r="F4">
         <v>30000</v>
       </c>
@@ -3337,8 +3732,11 @@
       <c r="I4" s="1">
         <v>12007880</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4">
+        <v>804000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>40000</v>
       </c>
@@ -3351,6 +3749,9 @@
       <c r="D5">
         <v>2530690</v>
       </c>
+      <c r="E5">
+        <v>875880</v>
+      </c>
       <c r="F5">
         <v>40000</v>
       </c>
@@ -3363,8 +3764,11 @@
       <c r="I5" s="1">
         <v>15451910</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5">
+        <v>1076130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50000</v>
       </c>
@@ -3377,6 +3781,9 @@
       <c r="D6">
         <v>2695580</v>
       </c>
+      <c r="E6">
+        <v>1416290</v>
+      </c>
       <c r="F6">
         <v>50000</v>
       </c>
@@ -3389,8 +3796,11 @@
       <c r="I6" s="1">
         <v>20897770</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6">
+        <v>3365950</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>60000</v>
       </c>
@@ -3403,6 +3813,9 @@
       <c r="D7">
         <v>3460310</v>
       </c>
+      <c r="E7">
+        <v>1477660</v>
+      </c>
       <c r="F7">
         <v>60000</v>
       </c>
@@ -3415,8 +3828,11 @@
       <c r="I7" s="1">
         <v>28535280</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7">
+        <v>2465300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>70000</v>
       </c>
@@ -3429,6 +3845,9 @@
       <c r="D8">
         <v>3672300</v>
       </c>
+      <c r="E8">
+        <v>1823040</v>
+      </c>
       <c r="F8">
         <v>70000</v>
       </c>
@@ -3441,8 +3860,11 @@
       <c r="I8" s="1">
         <v>35879390</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8">
+        <v>3141570</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>80000</v>
       </c>
@@ -3455,6 +3877,9 @@
       <c r="D9">
         <v>4668330</v>
       </c>
+      <c r="E9">
+        <v>2197880</v>
+      </c>
       <c r="F9">
         <v>80000</v>
       </c>
@@ -3467,8 +3892,11 @@
       <c r="I9" s="1">
         <v>43015550</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9">
+        <v>2240380</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>90000</v>
       </c>
@@ -3481,6 +3909,9 @@
       <c r="D10">
         <v>7091910</v>
       </c>
+      <c r="E10">
+        <v>2303450</v>
+      </c>
       <c r="F10">
         <v>90000</v>
       </c>
@@ -3493,8 +3924,11 @@
       <c r="I10" s="1">
         <v>48911090</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10">
+        <v>2467080</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>100000</v>
       </c>
@@ -3507,6 +3941,9 @@
       <c r="D11">
         <v>6365950</v>
       </c>
+      <c r="E11">
+        <v>2539160</v>
+      </c>
       <c r="F11">
         <v>100000</v>
       </c>
@@ -3519,8 +3956,11 @@
       <c r="I11" s="1">
         <v>58858030</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11">
+        <v>2847210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>110000</v>
       </c>
@@ -3533,6 +3973,9 @@
       <c r="D12" s="1">
         <v>10200350</v>
       </c>
+      <c r="E12">
+        <v>3487350</v>
+      </c>
       <c r="F12">
         <v>110000</v>
       </c>
@@ -3545,8 +3988,11 @@
       <c r="I12" s="1">
         <v>68348030</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12">
+        <v>7391610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>120000</v>
       </c>
@@ -3559,6 +4005,9 @@
       <c r="D13">
         <v>8711210</v>
       </c>
+      <c r="E13">
+        <v>3960920</v>
+      </c>
       <c r="F13">
         <v>120000</v>
       </c>
@@ -3571,8 +4020,11 @@
       <c r="I13" s="1">
         <v>77035280</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13">
+        <v>4860750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>130000</v>
       </c>
@@ -3585,6 +4037,9 @@
       <c r="D14" s="1">
         <v>10598160</v>
       </c>
+      <c r="E14">
+        <v>5314110</v>
+      </c>
       <c r="F14">
         <v>130000</v>
       </c>
@@ -3597,8 +4052,11 @@
       <c r="I14" s="1">
         <v>87388400</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14">
+        <v>4207670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>140000</v>
       </c>
@@ -3611,6 +4069,9 @@
       <c r="D15">
         <v>9733400</v>
       </c>
+      <c r="E15">
+        <v>4837220</v>
+      </c>
       <c r="F15">
         <v>140000</v>
       </c>
@@ -3623,8 +4084,11 @@
       <c r="I15" s="1">
         <v>124880320</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15">
+        <v>6618730</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>150000</v>
       </c>
@@ -3637,6 +4101,9 @@
       <c r="D16" s="1">
         <v>12286210</v>
       </c>
+      <c r="E16">
+        <v>4866130</v>
+      </c>
       <c r="F16">
         <v>150000</v>
       </c>
@@ -3649,8 +4116,11 @@
       <c r="I16" s="1">
         <v>135442330</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16">
+        <v>6678270</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>160000</v>
       </c>
@@ -3663,6 +4133,9 @@
       <c r="D17" s="1">
         <v>17591560</v>
       </c>
+      <c r="E17">
+        <v>5441180</v>
+      </c>
       <c r="F17">
         <v>160000</v>
       </c>
@@ -3675,8 +4148,11 @@
       <c r="I17" s="1">
         <v>140489320</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17">
+        <v>7236720</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>170000</v>
       </c>
@@ -3689,6 +4165,9 @@
       <c r="D18" s="1">
         <v>16782940</v>
       </c>
+      <c r="E18">
+        <v>6135550</v>
+      </c>
       <c r="F18">
         <v>170000</v>
       </c>
@@ -3701,8 +4180,11 @@
       <c r="I18" s="1">
         <v>156968140</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="1">
+        <v>13946480</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>180000</v>
       </c>
@@ -3715,6 +4197,9 @@
       <c r="D19" s="1">
         <v>22357220</v>
       </c>
+      <c r="E19">
+        <v>7186640</v>
+      </c>
       <c r="F19">
         <v>180000</v>
       </c>
@@ -3727,8 +4212,11 @@
       <c r="I19" s="1">
         <v>167732350</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19">
+        <v>7553610</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>190000</v>
       </c>
@@ -3741,6 +4229,9 @@
       <c r="D20" s="1">
         <v>29298090</v>
       </c>
+      <c r="E20">
+        <v>6822590</v>
+      </c>
       <c r="F20">
         <v>190000</v>
       </c>
@@ -3753,8 +4244,11 @@
       <c r="I20" s="1">
         <v>197140190</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20">
+        <v>9107510</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>200000</v>
       </c>
@@ -3767,6 +4261,9 @@
       <c r="D21" s="1">
         <v>29363270</v>
       </c>
+      <c r="E21">
+        <v>7430620</v>
+      </c>
       <c r="F21">
         <v>200000</v>
       </c>
@@ -3779,6 +4276,15 @@
       <c r="I21" s="1">
         <v>201503280</v>
       </c>
+      <c r="J21" s="1">
+        <v>10107810</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D44" s="1"/>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.35">
       <c r="J81" s="1"/>

</xml_diff>